<commit_message>
change folder name, done report, link video
</commit_message>
<xml_diff>
--- a/Report/Team3 - CLC02 - Prj Contribution.xlsx
+++ b/Report/Team3 - CLC02 - Prj Contribution.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MinhTran\Downloads\Download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\HK2_22-23\KTLT\group-project\CSC10002-Group-A-Course-Management-System\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3584CFD7-CEE0-4DC8-A3A1-70B729BA95D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3CF094-513B-49E1-B848-7EEE5F7B6045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -516,22 +516,6 @@
     <xf numFmtId="9" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -566,14 +550,36 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -584,14 +590,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2714,6 +2714,94 @@
         <a:xfrm>
           <a:off x="6117167" y="9980084"/>
           <a:ext cx="4545978" cy="645583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>69695</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>46464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2369634</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>22108</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0507FBC-EC63-1ABB-3432-D83DEA2103BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6040244" y="25973049"/>
+          <a:ext cx="2299939" cy="556437"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>41586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2485793</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>533474</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A14E325F-F69B-B6D6-11C5-E03855BAEF7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5970550" y="7150488"/>
+          <a:ext cx="2485792" cy="491888"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2928,8 +3016,8 @@
   </sheetPr>
   <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="A50" zoomScale="108" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2972,15 +3060,15 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="16"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="3"/>
@@ -3059,33 +3147,33 @@
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4890,1126 +4978,1126 @@
   </sheetPr>
   <dimension ref="A1:F992"/>
   <sheetViews>
-    <sheetView zoomScale="41" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="41" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.5703125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" style="22" customWidth="1"/>
-    <col min="6" max="6" width="100.140625" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="12.5703125" style="22"/>
+    <col min="1" max="2" width="12.5703125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="100.140625" style="14" customWidth="1"/>
+    <col min="7" max="16384" width="12.5703125" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="41" t="s">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="23"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25">
+      <c r="A4" s="17">
         <v>1</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="17">
         <v>22127026</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="17">
         <v>5</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="23" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25">
+      <c r="A5" s="17">
         <v>2</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="17">
         <v>22127026</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="17">
         <v>10</v>
       </c>
-      <c r="F5" s="25"/>
+      <c r="F5" s="17"/>
     </row>
     <row r="6" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25">
+      <c r="A6" s="17">
         <v>3</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="17">
         <v>22127026</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="17">
         <v>10</v>
       </c>
-      <c r="F6" s="25"/>
+      <c r="F6" s="17"/>
     </row>
     <row r="7" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25">
+      <c r="A7" s="17">
         <v>4</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="17">
         <v>22127026</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="17">
         <v>10</v>
       </c>
-      <c r="F7" s="25"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25">
+      <c r="A8" s="17">
         <v>5</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="17">
         <v>22127026</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="17">
         <v>11</v>
       </c>
-      <c r="F8" s="25"/>
+      <c r="F8" s="17"/>
     </row>
     <row r="9" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25">
+      <c r="A9" s="17">
         <v>6</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="17">
         <v>22127026</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="17">
         <v>8</v>
       </c>
-      <c r="F9" s="25"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25">
+      <c r="A10" s="17">
         <v>7</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="17">
         <v>22127026</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="17">
         <v>8</v>
       </c>
-      <c r="F10" s="25"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25">
+      <c r="A11" s="17">
         <v>8</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="17">
         <v>22127026</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="17">
         <v>1</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25">
+      <c r="A12" s="17">
         <v>9</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="17">
         <v>22127026</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="17">
         <v>15</v>
       </c>
-      <c r="F12" s="25"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25">
+      <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="17">
         <v>22127026</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="17">
         <v>5</v>
       </c>
-      <c r="F13" s="25"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27">
+      <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="19">
         <v>22127123</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="19">
         <v>5</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="25" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27">
+      <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="19">
         <v>22127123</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="19">
         <v>5</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="26" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27">
+      <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="19">
         <v>22127123</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="19">
         <v>3</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="25" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27">
+      <c r="A17" s="19">
         <v>14</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="19">
         <v>22127123</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="19">
         <v>5</v>
       </c>
-      <c r="F17" s="27"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27">
+      <c r="A18" s="19">
         <v>15</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="19">
         <v>22127123</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="D18" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="19">
         <v>4</v>
       </c>
-      <c r="F18" s="27"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27">
+      <c r="A19" s="19">
         <v>16</v>
       </c>
-      <c r="B19" s="27">
+      <c r="B19" s="19">
         <v>22127123</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="19">
         <v>9</v>
       </c>
-      <c r="F19" s="27"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27">
+      <c r="A20" s="19">
         <v>17</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="19">
         <v>22127123</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="19">
         <v>7</v>
       </c>
-      <c r="F20" s="27"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27">
+      <c r="A21" s="19">
         <v>18</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="19">
         <v>22127123</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="19">
         <v>2</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="28" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="27">
+      <c r="A22" s="19">
         <v>19</v>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="19">
         <v>22127123</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="19">
         <v>20</v>
       </c>
-      <c r="F22" s="27"/>
+      <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27">
+      <c r="A23" s="19">
         <v>20</v>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="19">
         <v>22127123</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="19">
         <v>30</v>
       </c>
-      <c r="F23" s="27"/>
+      <c r="F23" s="19"/>
     </row>
     <row r="24" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="29">
+      <c r="A24" s="21">
         <v>21</v>
       </c>
-      <c r="B24" s="29">
+      <c r="B24" s="21">
         <v>22127275</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="21">
         <v>6</v>
       </c>
-      <c r="F24" s="37"/>
+      <c r="F24" s="39"/>
     </row>
     <row r="25" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29">
+      <c r="A25" s="21">
         <v>22</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="21">
         <v>22127275</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="21">
         <v>4</v>
       </c>
-      <c r="F25" s="39"/>
+      <c r="F25" s="41"/>
     </row>
     <row r="26" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29">
+      <c r="A26" s="21">
         <v>23</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B26" s="21">
         <v>22127275</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="21">
         <v>7</v>
       </c>
-      <c r="F26" s="37"/>
+      <c r="F26" s="39"/>
     </row>
     <row r="27" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29">
+      <c r="A27" s="21">
         <v>24</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B27" s="21">
         <v>22127275</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="21">
         <v>6</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
     </row>
     <row r="28" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29">
+      <c r="A28" s="21">
         <v>25</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="21">
         <v>22127275</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="29">
+      <c r="E28" s="21">
         <v>8</v>
       </c>
-      <c r="F28" s="29"/>
+      <c r="F28" s="21"/>
     </row>
     <row r="29" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29">
+      <c r="A29" s="21">
         <v>26</v>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="21">
         <v>22127275</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="29">
+      <c r="E29" s="21">
         <v>7</v>
       </c>
-      <c r="F29" s="37"/>
+      <c r="F29" s="39"/>
     </row>
     <row r="30" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29">
+      <c r="A30" s="21">
         <v>27</v>
       </c>
-      <c r="B30" s="29">
+      <c r="B30" s="21">
         <v>22127275</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="29">
+      <c r="E30" s="21">
         <v>7</v>
       </c>
-      <c r="F30" s="38"/>
+      <c r="F30" s="40"/>
     </row>
     <row r="31" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="29">
+      <c r="A31" s="21">
         <v>28</v>
       </c>
-      <c r="B31" s="29">
+      <c r="B31" s="21">
         <v>22127275</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="21">
         <v>6</v>
       </c>
-      <c r="F31" s="39"/>
+      <c r="F31" s="41"/>
     </row>
     <row r="32" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="29">
+      <c r="A32" s="21">
         <v>29</v>
       </c>
-      <c r="B32" s="29">
+      <c r="B32" s="21">
         <v>22127275</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="29">
+      <c r="E32" s="21">
         <v>8</v>
       </c>
-      <c r="F32" s="29"/>
+      <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="29">
+      <c r="A33" s="21">
         <v>30</v>
       </c>
-      <c r="B33" s="29">
+      <c r="B33" s="21">
         <v>22127275</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="29">
+      <c r="E33" s="21">
         <v>30</v>
       </c>
-      <c r="F33" s="29"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="30">
+      <c r="A34" s="22">
         <v>31</v>
       </c>
-      <c r="B34" s="30">
+      <c r="B34" s="22">
         <v>22127402</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="22">
         <v>10</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30">
+      <c r="A35" s="22">
         <v>32</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B35" s="22">
         <v>22127402</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E35" s="22">
         <v>10</v>
       </c>
-      <c r="F35" s="35"/>
+      <c r="F35" s="38"/>
     </row>
     <row r="36" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="30">
+      <c r="A36" s="22">
         <v>33</v>
       </c>
-      <c r="B36" s="30">
+      <c r="B36" s="22">
         <v>22127402</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="22">
         <v>8</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="37"/>
     </row>
     <row r="37" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="30">
+      <c r="A37" s="22">
         <v>34</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B37" s="22">
         <v>22127402</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="22">
         <v>8</v>
       </c>
-      <c r="F37" s="35"/>
+      <c r="F37" s="38"/>
     </row>
     <row r="38" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="30">
+      <c r="A38" s="22">
         <v>35</v>
       </c>
-      <c r="B38" s="30">
+      <c r="B38" s="22">
         <v>22127402</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="30">
+      <c r="E38" s="22">
         <v>7</v>
       </c>
-      <c r="F38" s="34"/>
+      <c r="F38" s="37"/>
     </row>
     <row r="39" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="30">
+      <c r="A39" s="22">
         <v>36</v>
       </c>
-      <c r="B39" s="30">
+      <c r="B39" s="22">
         <v>22127402</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="30">
+      <c r="E39" s="22">
         <v>7</v>
       </c>
-      <c r="F39" s="35"/>
+      <c r="F39" s="38"/>
     </row>
     <row r="40" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="30">
+      <c r="A40" s="22">
         <v>37</v>
       </c>
-      <c r="B40" s="30">
+      <c r="B40" s="22">
         <v>22127402</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="30">
+      <c r="E40" s="22">
         <v>1</v>
       </c>
-      <c r="F40" s="30"/>
+      <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="30">
+      <c r="A41" s="22">
         <v>38</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B41" s="22">
         <v>22127402</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="30">
+      <c r="E41" s="22">
         <v>1</v>
       </c>
-      <c r="F41" s="30"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30">
+      <c r="A42" s="22">
         <v>39</v>
       </c>
-      <c r="B42" s="30">
+      <c r="B42" s="22">
         <v>22127402</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="E42" s="30">
+      <c r="E42" s="22">
         <v>24</v>
       </c>
-      <c r="F42" s="30"/>
+      <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="30">
+      <c r="A43" s="22">
         <v>40</v>
       </c>
-      <c r="B43" s="30">
+      <c r="B43" s="22">
         <v>22127402</v>
       </c>
-      <c r="C43" s="30" t="s">
+      <c r="C43" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D43" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E43" s="30">
+      <c r="E43" s="22">
         <v>2</v>
       </c>
-      <c r="F43" s="30"/>
+      <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
     </row>
     <row r="45" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
     </row>
     <row r="46" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
     </row>
     <row r="47" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="24"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
     </row>
     <row r="48" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="24"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
     </row>
     <row r="49" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="24"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
     </row>
     <row r="51" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
+      <c r="A51" s="16"/>
+      <c r="B51" s="16"/>
     </row>
     <row r="52" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
     </row>
     <row r="53" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
     </row>
     <row r="54" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="16"/>
     </row>
     <row r="55" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
     </row>
     <row r="56" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="24"/>
-      <c r="B56" s="24"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="16"/>
     </row>
     <row r="57" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="24"/>
-      <c r="B57" s="24"/>
+      <c r="A57" s="16"/>
+      <c r="B57" s="16"/>
     </row>
     <row r="58" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="16"/>
     </row>
     <row r="59" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
+      <c r="A59" s="16"/>
+      <c r="B59" s="16"/>
     </row>
     <row r="60" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="16"/>
     </row>
     <row r="61" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24"/>
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
     </row>
     <row r="62" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="24"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
     </row>
     <row r="63" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="24"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
+      <c r="A63" s="16"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
     </row>
     <row r="64" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="24"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
     </row>
     <row r="65" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="24"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
     </row>
     <row r="66" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="24"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="16"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
     </row>
     <row r="67" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="24"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
+      <c r="A67" s="16"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
     </row>
     <row r="68" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="24"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
+      <c r="A68" s="16"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
     </row>
     <row r="69" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="24"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
     </row>
     <row r="70" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="24"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
     </row>
     <row r="71" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="24"/>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
     </row>
     <row r="72" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="24"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
     </row>
     <row r="73" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="24"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
     </row>
     <row r="74" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="24"/>
-      <c r="B74" s="24"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
     </row>
     <row r="75" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="24"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
     </row>
     <row r="76" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="24"/>
-      <c r="B76" s="24"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
+      <c r="A76" s="16"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
     </row>
     <row r="77" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="24"/>
-      <c r="B77" s="24"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
+      <c r="A77" s="16"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16"/>
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
     </row>
     <row r="78" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="24"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
+      <c r="A78" s="16"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
     </row>
     <row r="79" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="24"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
     </row>
     <row r="80" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="24"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
+      <c r="A80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
     </row>
     <row r="81" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="24"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
+      <c r="A81" s="16"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
     </row>
     <row r="82" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="24"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
     </row>
     <row r="83" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="24"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
+      <c r="A83" s="16"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
     </row>
     <row r="84" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="24"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
+      <c r="A84" s="16"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
     </row>
     <row r="85" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="24"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
+      <c r="A85" s="16"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="16"/>
     </row>
     <row r="86" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="24"/>
-      <c r="B86" s="24"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
+      <c r="A86" s="16"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
     </row>
     <row r="87" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="24"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
+      <c r="A87" s="16"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
     </row>
     <row r="88" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="24"/>
-      <c r="B88" s="24"/>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
+      <c r="A88" s="16"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
     </row>
     <row r="89" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="24"/>
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="16"/>
+      <c r="E89" s="16"/>
+      <c r="F89" s="16"/>
     </row>
     <row r="90" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="24"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
+      <c r="A90" s="16"/>
+      <c r="B90" s="16"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
     </row>
     <row r="91" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="24"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
+      <c r="A91" s="16"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="16"/>
+      <c r="D91" s="16"/>
+      <c r="E91" s="16"/>
+      <c r="F91" s="16"/>
     </row>
     <row r="92" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="24"/>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
+      <c r="A92" s="16"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="16"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="16"/>
+      <c r="F92" s="16"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>